<commit_message>
Raw data - summary
</commit_message>
<xml_diff>
--- a/LifeChem raw data/DENV_RdRp_LifeChem_Selected from HTS.xlsx
+++ b/LifeChem raw data/DENV_RdRp_LifeChem_Selected from HTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/uccaris_ucl_ac_uk/Documents/GitHub/CNP11-DENVRdrp-LifeChem/LifeChem raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{7695B862-A956-4572-92BA-1E60C5DF7F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA8812FC-9992-456B-A003-2293D9B579A5}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{7695B862-A956-4572-92BA-1E60C5DF7F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37A1DF9E-0B5A-4BCB-812C-2424235ABC82}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1486,12 +1486,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D65"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update DENV_RdRp_LifeChem_Selected from HTS.xlsx
</commit_message>
<xml_diff>
--- a/LifeChem raw data/DENV_RdRp_LifeChem_Selected from HTS.xlsx
+++ b/LifeChem raw data/DENV_RdRp_LifeChem_Selected from HTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/uccaris_ucl_ac_uk/Documents/GitHub/CNP11-DENVRdrp-LifeChem/LifeChem raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{7695B862-A956-4572-92BA-1E60C5DF7F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37A1DF9E-0B5A-4BCB-812C-2424235ABC82}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{7695B862-A956-4572-92BA-1E60C5DF7F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1FECCCF-9C04-49A1-B96B-507C8FF1C017}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1188,9 +1188,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1228,7 +1228,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1334,7 +1334,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1476,7 +1476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1486,13 +1486,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>